<commit_message>
modify try and catch block
</commit_message>
<xml_diff>
--- a/Invoice_Record.xlsx
+++ b/Invoice_Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shubham\Desktop\RPA\MyProjects\Calculator Demo\My First Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DF9630-09C9-4819-9BEB-92D9AA9CAF55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D154DC7-8A00-4A88-91D3-729F6C3DF690}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="2820" windowWidth="15375" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -349,10 +349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B7"/>
+      <selection activeCell="A2" sqref="A2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,35 +383,38 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>850778</v>
+        <v>859988</v>
       </c>
       <c r="B4" s="1">
-        <v>5000</v>
+        <v>4890</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>859988</v>
+        <v>820988</v>
       </c>
       <c r="B5" s="1">
-        <v>4890</v>
+        <v>4241</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>820988</v>
+        <v>80000</v>
       </c>
       <c r="B6" s="1">
-        <v>4241</v>
+        <v>9940.99</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>80000</v>
+        <v>850778</v>
       </c>
       <c r="B7" s="1">
-        <v>9940.99</v>
-      </c>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>